<commit_message>
tuned the paramaters of Admittance control, auto-label v-state
</commit_message>
<xml_diff>
--- a/A_User/Record/HRC参数调试记录.xlsx
+++ b/A_User/Record/HRC参数调试记录.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
   <si>
     <t>size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,12 +252,98 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">k_cartesian = diag([100,100,100*2,0,0,0]*1*1)*1.3*5*2*1.5/2
+b_cartesian = diag([100,100,100*2*1.7,0,0,0]*14*0.707*45/1000*0.7*5*1.4/2*1.4)
+H_inv          = diag([1,1,1/4,0,0,0]/10/5*3)  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ts = 0.015;
+Kp_joint = eye(7)*0;    %比例控制系数3
+k0 =  0.00003;            %障碍物斥力系数 
+FUTURE=3;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if obs &lt;=66
+    center(3)=center(3)-0.0;
+else
+    center(3)=center(3)+0.0;
+end</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size=cell2mat(myspace(obs,2));
+size(1)=size(1)/2;
+size(2)=size(2)/2;
+expand=0.1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.09.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导纳参数  主程序.m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主程序.m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>find_distance.m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>现象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空载可以，加上IMU不行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k_cartesian = diag([100,100,100,0,0,0])*3;  
+b_cartesian = diag([100,100,100,0,0,0]*1.5);
+H_inv          = diag([1,1,1,0,0,0]/10/5*3)   ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timex = 5; %运行时间系数
+Ts = 0.01;
+Kp_joint = eye(7)*0;    %比例控制系数3
+k0 =  0.00005;            %障碍物斥力系数 
+FUTURE=3;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if obs &lt;=66
+    center(3)=center(3)-0.0;
+else
+    center(3)=center(3)+0.05;
+end</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.09.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加上IMU也可以</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,6 +442,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,11 +728,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="13" style="2" customWidth="1"/>
@@ -655,7 +745,7 @@
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:8" ht="20.25">
+    <row r="6" spans="2:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -698,7 +788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -718,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -738,7 +828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -758,7 +848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -778,7 +868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
@@ -798,7 +888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -818,7 +908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
@@ -838,7 +928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -861,7 +951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
@@ -884,7 +974,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
@@ -904,7 +994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -924,7 +1014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>11</v>
       </c>
@@ -944,7 +1034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="4" customFormat="1">
+    <row r="20" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
@@ -964,7 +1054,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
@@ -987,7 +1077,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1007,7 +1097,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1050,7 +1140,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>11</v>
       </c>
@@ -1092,7 +1182,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>11</v>
       </c>
@@ -1115,7 +1205,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>11</v>
       </c>
@@ -1138,7 +1228,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>11</v>
       </c>
@@ -1161,7 +1251,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>11</v>
       </c>
@@ -1184,7 +1274,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:8" s="4" customFormat="1">
+    <row r="31" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>11</v>
       </c>
@@ -1207,7 +1297,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:8" s="4" customFormat="1">
+    <row r="32" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
@@ -1230,7 +1320,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1">
+    <row r="33" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>37</v>
       </c>
@@ -1253,7 +1343,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="4" customFormat="1">
+    <row r="34" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
         <v>11</v>
       </c>
@@ -1276,7 +1366,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="54">
+    <row r="35" spans="1:8" ht="54" x14ac:dyDescent="0.2">
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1287,7 +1377,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>46</v>
       </c>
@@ -1310,7 +1400,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1">
+    <row r="37" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>50</v>
       </c>
@@ -1333,9 +1423,93 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="24.75" customHeight="1">
+    <row r="38" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="57.75" customWidth="1"/>
+    <col min="2" max="2" width="37.875" customWidth="1"/>
+    <col min="3" max="3" width="28.875" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
loop_over update FUTURE; RL2m3m3_maze_big modify R; get_init_big_maze_v1 modify map
</commit_message>
<xml_diff>
--- a/A_User/Record/HRC参数调试记录.xlsx
+++ b/A_User/Record/HRC参数调试记录.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
   <si>
     <t>size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -338,12 +339,48 @@
     <t>加上IMU也可以</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>yang's 导纳参数；计算机器人本体斥力；不加IMU；不计算障碍物斥力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以跑完；但会碰到第五个障碍物</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单导纳参数；计算机器人本体斥力；不加IMU；不计算障碍物斥力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以跑完；但会碰到第五个障碍物；在终点处有徘徊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yang's 导纳参数；计算机器人本体斥力；加IMU；不计算障碍物斥力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四五障碍物间超限辐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单导纳参数；计算机器人本体斥力；加IMU；不计算障碍物斥力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单导纳参数；计算机器人本体斥力；加IMU；不计算障碍物斥力，同时将pos_table同步为末端位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yang's 导纳参数；计算机器人本体斥力；加IMU；不计算障碍物斥力，同时将pos_table同步为末端位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -732,7 +769,7 @@
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="13" style="2" customWidth="1"/>
@@ -745,7 +782,7 @@
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:8" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" ht="20.25">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -788,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -808,7 +845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -828,7 +865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -848,7 +885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -868,7 +905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
@@ -888,7 +925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -908,7 +945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8">
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
@@ -928,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8">
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -951,7 +988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8">
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
@@ -974,7 +1011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8">
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
@@ -994,7 +1031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8">
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1014,7 +1051,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8">
       <c r="B19" s="2" t="s">
         <v>11</v>
       </c>
@@ -1034,7 +1071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" s="4" customFormat="1">
       <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1054,7 +1091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8">
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1077,7 +1114,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8">
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1097,7 +1134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1120,7 +1157,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8">
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1140,7 +1177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8">
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
@@ -1161,7 +1198,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8">
       <c r="B26" s="5" t="s">
         <v>11</v>
       </c>
@@ -1182,7 +1219,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8">
       <c r="B27" s="5" t="s">
         <v>11</v>
       </c>
@@ -1205,7 +1242,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8">
       <c r="B28" s="5" t="s">
         <v>11</v>
       </c>
@@ -1228,7 +1265,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8">
       <c r="B29" s="5" t="s">
         <v>11</v>
       </c>
@@ -1251,7 +1288,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8">
       <c r="B30" s="5" t="s">
         <v>11</v>
       </c>
@@ -1274,7 +1311,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" s="4" customFormat="1">
       <c r="B31" s="4" t="s">
         <v>11</v>
       </c>
@@ -1297,7 +1334,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" s="4" customFormat="1">
       <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
@@ -1320,7 +1357,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="4" customFormat="1">
       <c r="B33" s="4" t="s">
         <v>37</v>
       </c>
@@ -1343,7 +1380,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" s="4" customFormat="1">
       <c r="B34" s="4" t="s">
         <v>11</v>
       </c>
@@ -1366,7 +1403,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="54" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="54">
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1377,7 +1414,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="B36" s="2" t="s">
         <v>46</v>
       </c>
@@ -1400,7 +1437,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" s="4" customFormat="1">
       <c r="B37" s="4" t="s">
         <v>50</v>
       </c>
@@ -1423,7 +1460,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="24.75" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -1439,11 +1476,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="57.75" customWidth="1"/>
     <col min="2" max="2" width="37.875" customWidth="1"/>
@@ -1452,7 +1489,7 @@
     <col min="5" max="5" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1472,7 +1509,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="88.5" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
@@ -1492,7 +1529,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="103.5" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -1510,6 +1547,75 @@
       </c>
       <c r="F3" s="8" t="s">
         <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="95.25" customWidth="1"/>
+    <col min="2" max="2" width="44.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>